<commit_message>
POCOR-6680: code enhance in students report cards | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/student_profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/student_profile_template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="131">
   <si>
     <t>${Institutions.name}/${Institutions.code}</t>
   </si>
@@ -407,6 +407,18 @@
   </si>
   <si>
     <t>${"match": {"displayValue": "UserContacts.contact","rows": {"matchFrom": "UserContacts.id","matchTo": "UserContacts.id"}}}</t>
+  </si>
+  <si>
+    <t>Mother Name :</t>
+  </si>
+  <si>
+    <t>${StudentMoterDetails.mother_name}</t>
+  </si>
+  <si>
+    <t>Mother Contact :</t>
+  </si>
+  <si>
+    <t>${StudentMoterDetails.mother_contact}</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1330,8 +1342,24 @@
       <c r="E49" s="19"/>
     </row>
     <row r="50" spans="3:5" ht="12.75" customHeight="1"/>
-    <row r="51" spans="3:5" ht="12.75" customHeight="1"/>
-    <row r="52" spans="3:5" ht="12.75" customHeight="1"/>
+    <row r="51" spans="3:5" ht="12.75" customHeight="1">
+      <c r="C51" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51" s="20"/>
+    </row>
+    <row r="52" spans="3:5" ht="12.75" customHeight="1">
+      <c r="C52" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E52" s="20"/>
+    </row>
     <row r="53" spans="3:5" ht="12.75" customHeight="1"/>
     <row r="54" spans="3:5" ht="12.75" customHeight="1"/>
     <row r="55" spans="3:5" ht="12.75" customHeight="1"/>
@@ -2280,7 +2308,10 @@
     <row r="998" ht="12.75" customHeight="1"/>
     <row r="999" ht="12.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="28">
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="D36:E36"/>
@@ -2291,6 +2322,7 @@
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D51:E51"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
@@ -2305,8 +2337,6 @@
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
POCOR-7316|Develop transcript and award placeholder|Status:Complete
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/student_profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/student_profile_template.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\pocor-openemis-core\webroot\export\customexcel\default_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EABD84D-B1CB-4BE4-AF39-BF01D05D94B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9F3272-EA70-4E4F-B483-95834C3BD594}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="10" r:id="rId2"/>
+    <sheet name="Transcript" sheetId="10" r:id="rId2"/>
     <sheet name="Risks" sheetId="2" r:id="rId3"/>
     <sheet name="Classes" sheetId="3" r:id="rId4"/>
     <sheet name="Co-curricular" sheetId="4" r:id="rId5"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="152">
   <si>
     <t>${Institutions.name}/${Institutions.code}</t>
   </si>
@@ -432,18 +432,6 @@
     <t>Student Awards</t>
   </si>
   <si>
-    <t>${StudentAwards1.date}</t>
-  </si>
-  <si>
-    <t>${StudentAwards1.name}</t>
-  </si>
-  <si>
-    <t>${StudentAwards2.date}</t>
-  </si>
-  <si>
-    <t>${StudentAwards2.name}</t>
-  </si>
-  <si>
     <t>Academic Periods</t>
   </si>
   <si>
@@ -465,31 +453,37 @@
     <t>GPA</t>
   </si>
   <si>
-    <t xml:space="preserve">${Assessments.academic_period.name} </t>
-  </si>
-  <si>
-    <t>${EducationProgramme.Name}</t>
-  </si>
-  <si>
-    <t>${EducationGrade.Name}</t>
-  </si>
-  <si>
     <t>${"match": {"displayValue": "InstitutionSubjectStudentsWithName.name","rows": {"matchFrom": "InstitutionSubjectStudentsWithName.id","matchTo": "InstitutionSubjectStudentsWithName.id"}}}</t>
   </si>
   <si>
     <t>${"match": {"displayValue": "InstitutionSubjectStudentsWithName.subjectName","rows": {"matchFrom": "InstitutionSubjectStudentsWithName.id","matchTo": "InstitutionSubjectStudentsWithName.id"}}}</t>
   </si>
   <si>
-    <t>${"match": {"displayValue": "AssessmentItemResults.marks_formatted","type":"number","format":"2","rows": {"matchFrom": "InstitutionSubjectStudentsWithName.education_subject_id","matchTo": "AssessmentItemResults.education_subject_id"},"columns": {"matchFrom": "AssessmentPeriods.id","matchTo": "AssessmentItemResults.assessment_period_id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "InstitutionSubjectStudents.total_mark","type":"number","format":"2","rows": {"matchFrom": "InstitutionSubjectStudentsWithName.education_subject_id","matchTo": "InstitutionSubjectStudentsWithName.education_subject_id"}}}</t>
-  </si>
-  <si>
     <t>{studentGPA}</t>
   </si>
   <si>
     <t>${Institutions.area}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionSubjectStudentsWithName.academic_period_name","rows": {"matchFrom": "InstitutionSubjectStudentsWithName.id","matchTo": "InstitutionSubjectStudentsWithName.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionSubjectStudentsWithName.education_programme_name","rows": {"matchFrom": "InstitutionSubjectStudentsWithName.id","matchTo": "InstitutionSubjectStudentsWithName.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionSubjectStudentsWithName.education_grade_name","rows": {"matchFrom": "InstitutionSubjectStudentsWithName.id","matchTo": "InstitutionSubjectStudentsWithName.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "InstitutionSubjectStudentsWithName.total_mark","rows": {"matchFrom": "InstitutionSubjectStudentsWithName.id","matchTo": "InstitutionSubjectStudentsWithName.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "AssessmentItemResults.marks_formatted","type":"number","format":"2","rows": {"matchFrom": "InstitutionSubjectStudentsWithName.id","matchTo": "AssessmentItemResults.id"},"columns": {"matchFrom": "AssessmentPeriods.id","matchTo": "AssessmentItemResults.assessment_period_id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentAwards.date","rows": {"matchFrom": "StudentAwards.id","matchTo": "StudentAwards.id"}}}</t>
+  </si>
+  <si>
+    <t>${"match": {"displayValue": "StudentAwards.name","rows": {"matchFrom": "StudentAwards.id","matchTo": "StudentAwards.id"}}}</t>
   </si>
 </sst>
 </file>
@@ -591,7 +585,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -684,11 +678,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -742,7 +745,20 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -760,19 +776,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -785,6 +789,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1191,19 +1197,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F1006"/>
+  <dimension ref="A1:F1006"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35:E35"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="27" width="15.5703125" customWidth="1"/>
@@ -1213,167 +1219,167 @@
   <sheetData>
     <row r="1" spans="2:6" ht="12.75" customHeight="1"/>
     <row r="2" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="6" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
     </row>
     <row r="7" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
     </row>
     <row r="8" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
     </row>
     <row r="9" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
     </row>
     <row r="11" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
     </row>
     <row r="12" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
     </row>
     <row r="14" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="2:6" ht="12.75" customHeight="1">
       <c r="C15" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="16" spans="2:6" ht="12.75" customHeight="1">
       <c r="C16" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="E16" s="29"/>
+      <c r="E16" s="32"/>
     </row>
     <row r="17" spans="3:6" ht="12.75" customHeight="1">
       <c r="C17" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="E17" s="29"/>
+      <c r="E17" s="32"/>
     </row>
     <row r="18" spans="3:6" ht="12.75" customHeight="1">
       <c r="C18" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="E18" s="29"/>
+      <c r="E18" s="32"/>
     </row>
     <row r="19" spans="3:6" ht="12.75" customHeight="1">
       <c r="C19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="30"/>
     </row>
     <row r="20" spans="3:6" ht="12.75" customHeight="1">
       <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="35"/>
+      <c r="E20" s="30"/>
     </row>
     <row r="21" spans="3:6" ht="12.75" customHeight="1">
       <c r="C21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="35"/>
+      <c r="E21" s="30"/>
     </row>
     <row r="22" spans="3:6" ht="12.75" customHeight="1">
       <c r="C22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="35"/>
+      <c r="E22" s="30"/>
     </row>
     <row r="23" spans="3:6" ht="12.75" customHeight="1">
       <c r="C23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="35"/>
+      <c r="E23" s="30"/>
     </row>
     <row r="24" spans="3:6" ht="12.75" customHeight="1">
       <c r="C24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="35"/>
+      <c r="E24" s="30"/>
     </row>
     <row r="25" spans="3:6" ht="12.75" customHeight="1">
       <c r="C25" t="s">
@@ -1388,204 +1394,201 @@
       <c r="C26" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="35"/>
+      <c r="E26" s="30"/>
     </row>
     <row r="27" spans="3:6" ht="12.75" customHeight="1">
       <c r="C27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="35"/>
+      <c r="E27" s="30"/>
     </row>
     <row r="28" spans="3:6" ht="12.75" customHeight="1">
       <c r="C28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="35"/>
+      <c r="E28" s="30"/>
     </row>
     <row r="29" spans="3:6" ht="12.75" customHeight="1">
       <c r="C29" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="35"/>
+      <c r="E29" s="30"/>
     </row>
     <row r="30" spans="3:6" ht="12.75" customHeight="1">
       <c r="C30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="37"/>
+      <c r="E30" s="31"/>
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="3:6" s="19" customFormat="1" ht="12.75" customHeight="1">
       <c r="C31" s="22"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="3:6" s="19" customFormat="1" ht="12.75" customHeight="1">
       <c r="C32" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="E32" s="29"/>
+      <c r="E32" s="32"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="2:6" s="19" customFormat="1" ht="12.75" customHeight="1">
+    <row r="33" spans="1:6" s="19" customFormat="1" ht="12.75" customHeight="1">
       <c r="C33" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="D33" s="29" t="s">
+      <c r="D33" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="E33" s="29"/>
+      <c r="E33" s="32"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="2:6" s="19" customFormat="1" ht="12.75" customHeight="1">
+    <row r="34" spans="1:6" s="19" customFormat="1" ht="12.75" customHeight="1">
       <c r="C34" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="D34" s="29" t="s">
+      <c r="D34" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="E34" s="29"/>
+      <c r="E34" s="32"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="2:6" s="19" customFormat="1" ht="12.75" customHeight="1">
+    <row r="35" spans="1:6" s="19" customFormat="1" ht="12.75" customHeight="1">
       <c r="C35" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="D35" s="29" t="s">
-        <v>153</v>
+      <c r="D35" s="32" t="s">
+        <v>144</v>
       </c>
-      <c r="E35" s="29"/>
+      <c r="E35" s="32"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="2:6" s="19" customFormat="1" ht="12.75" customHeight="1">
+    <row r="36" spans="1:6" s="19" customFormat="1" ht="12.75" customHeight="1">
       <c r="C36"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="2:6" ht="15.75">
+    <row r="37" spans="1:6" ht="15.75">
       <c r="C37" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="D37" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="35"/>
-    </row>
-    <row r="38" spans="2:6" ht="12.75" customHeight="1">
+      <c r="E37" s="30"/>
+    </row>
+    <row r="38" spans="1:6" ht="12.75" customHeight="1">
       <c r="C38" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="35"/>
-    </row>
-    <row r="39" spans="2:6" ht="12.75" customHeight="1">
+      <c r="E38" s="30"/>
+    </row>
+    <row r="39" spans="1:6" ht="12.75" customHeight="1">
       <c r="C39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E39" s="35"/>
-    </row>
-    <row r="40" spans="2:6" ht="12.75" customHeight="1">
+      <c r="E39" s="30"/>
+    </row>
+    <row r="40" spans="1:6" ht="12.75" customHeight="1">
       <c r="C40" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="35" t="s">
+      <c r="D40" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E40" s="35"/>
-    </row>
-    <row r="41" spans="2:6" ht="12.75" customHeight="1">
+      <c r="E40" s="30"/>
+    </row>
+    <row r="41" spans="1:6" ht="12.75" customHeight="1">
       <c r="C41" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D41" s="35" t="s">
+      <c r="D41" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="35"/>
-    </row>
-    <row r="42" spans="2:6" ht="12.75" customHeight="1">
+      <c r="E41" s="30"/>
+    </row>
+    <row r="42" spans="1:6" ht="12.75" customHeight="1">
       <c r="C42" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D42" s="35" t="s">
+      <c r="D42" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E42" s="35"/>
-    </row>
-    <row r="43" spans="2:6" ht="12.75" customHeight="1">
+      <c r="E42" s="30"/>
+    </row>
+    <row r="43" spans="1:6" ht="12.75" customHeight="1">
       <c r="B43" s="23"/>
       <c r="C43" s="23"/>
       <c r="D43" s="23"/>
       <c r="E43" s="23"/>
       <c r="F43" s="23"/>
     </row>
-    <row r="44" spans="2:6">
+    <row r="44" spans="1:6">
       <c r="B44" s="25"/>
       <c r="C44" s="25"/>
       <c r="D44" s="25"/>
       <c r="E44" s="25"/>
       <c r="F44" s="25"/>
     </row>
-    <row r="45" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B45" s="31" t="s">
+    <row r="45" spans="1:6" ht="12.75" customHeight="1">
+      <c r="B45" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-    </row>
-    <row r="46" spans="2:6" ht="12.75" customHeight="1">
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+    </row>
+    <row r="46" spans="1:6" ht="12.75" customHeight="1">
       <c r="B46" s="25"/>
       <c r="C46" s="25"/>
       <c r="D46" s="25"/>
       <c r="E46" s="25"/>
       <c r="F46" s="25"/>
     </row>
-    <row r="47" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B47" s="25"/>
-      <c r="C47" s="24" t="s">
-        <v>134</v>
+    <row r="47" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A47" s="45"/>
+      <c r="B47" s="45"/>
+      <c r="C47" s="46" t="s">
+        <v>150</v>
       </c>
-      <c r="D47" s="29" t="s">
-        <v>135</v>
+      <c r="D47" s="32" t="s">
+        <v>151</v>
       </c>
-      <c r="E47" s="30"/>
+      <c r="E47" s="35"/>
       <c r="F47" s="25"/>
     </row>
-    <row r="48" spans="2:6" ht="12.75" customHeight="1">
+    <row r="48" spans="1:6" ht="12.75" customHeight="1">
       <c r="B48" s="25"/>
-      <c r="C48" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="D48" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="E48" s="30"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="35"/>
       <c r="F48" s="25"/>
     </row>
     <row r="49" ht="12.75" customHeight="1"/>
@@ -2548,25 +2551,6 @@
     <row r="1006" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="B45:F45"/>
@@ -2583,6 +2567,25 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D36:E36"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2608,33 +2611,34 @@
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="26" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C1" s="26" t="s">
         <v>46</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2648,19 +2652,19 @@
         <v>147</v>
       </c>
       <c r="D2" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="E2" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>151</v>
-      </c>
       <c r="H2" s="27" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="I2" s="28"/>
     </row>
@@ -2674,7 +2678,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2686,10 +2690,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="40"/>
+      <c r="B1" s="41"/>
     </row>
     <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="6" t="s">
@@ -2747,14 +2751,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
       <c r="A2" s="9" t="s">
@@ -3815,7 +3819,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0"/>
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -4865,7 +4871,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C989"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0"/>
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -4878,10 +4886,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="40"/>
+      <c r="B1" s="41"/>
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1">
       <c r="A2" s="12" t="s">
@@ -4919,10 +4927,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="40"/>
+      <c r="B7" s="41"/>
     </row>
     <row r="8" spans="1:3" ht="12.75" customHeight="1">
       <c r="A8" s="12" t="s">
@@ -5931,7 +5939,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0"/>
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -5945,15 +5955,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
@@ -33711,7 +33721,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D1001"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0"/>
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -33726,62 +33738,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="43"/>
+      <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="43"/>
+      <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="43" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="43"/>
+      <c r="D4" s="44"/>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="43" t="s">
+      <c r="B5" s="43"/>
+      <c r="C5" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="43"/>
+      <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="43" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="43"/>
+      <c r="D6" s="44"/>
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1">
       <c r="A8" s="6" t="s">
@@ -34805,17 +34817,17 @@
     <row r="1001" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -34844,12 +34856,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1">
       <c r="A2" s="6" t="s">

</xml_diff>

<commit_message>
POCOR-7316|fixed inprogress and marks |Status:Complete
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/student_profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/student_profile_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\pocor-openemis-core\webroot\export\customexcel\default_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9F3272-EA70-4E4F-B483-95834C3BD594}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF6EB40-29AF-4014-8FA6-862E09530782}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -585,7 +585,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -678,20 +678,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -736,9 +727,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -746,6 +734,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -759,9 +748,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -789,8 +775,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1197,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1006"/>
+  <dimension ref="A1:F1005"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1219,86 +1206,86 @@
   <sheetData>
     <row r="1" spans="2:6" ht="12.75" customHeight="1"/>
     <row r="2" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="6" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
     </row>
     <row r="7" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
     </row>
     <row r="9" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
     </row>
     <row r="10" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
     </row>
     <row r="11" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
     </row>
     <row r="12" spans="2:6" ht="12.75" customHeight="1">
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
     </row>
     <row r="14" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
     </row>
     <row r="15" spans="2:6" ht="12.75" customHeight="1">
       <c r="C15" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="E15" s="40"/>
+      <c r="E15" s="39"/>
     </row>
     <row r="16" spans="2:6" ht="12.75" customHeight="1">
       <c r="C16" s="20" t="s">
@@ -1550,47 +1537,41 @@
       <c r="F43" s="23"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
     </row>
     <row r="45" spans="1:6" ht="12.75" customHeight="1">
-      <c r="B45" s="36" t="s">
+      <c r="B45" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
     </row>
     <row r="46" spans="1:6" ht="12.75" customHeight="1">
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
     </row>
     <row r="47" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A47" s="45"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="46" t="s">
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="D47" s="32" t="s">
+      <c r="D47" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="E47" s="35"/>
-      <c r="F47" s="25"/>
-    </row>
-    <row r="48" spans="1:6" ht="12.75" customHeight="1">
-      <c r="B48" s="25"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="25"/>
-    </row>
+      <c r="E47" s="44"/>
+      <c r="F47" s="24"/>
+    </row>
+    <row r="48" spans="1:6" ht="12.75" customHeight="1"/>
     <row r="49" ht="12.75" customHeight="1"/>
     <row r="50" ht="12.75" customHeight="1"/>
     <row r="51" ht="12.75" customHeight="1"/>
@@ -2548,10 +2529,8 @@
     <row r="1003" ht="12.75" customHeight="1"/>
     <row r="1004" ht="12.75" customHeight="1"/>
     <row r="1005" ht="12.75" customHeight="1"/>
-    <row r="1006" ht="12.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="D48:E48"/>
+  <mergeCells count="34">
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="B45:F45"/>
     <mergeCell ref="B2:F2"/>
@@ -2616,57 +2595,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="25" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="I2" s="28"/>
+      <c r="I2" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2690,10 +2669,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="40"/>
     </row>
     <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="6" t="s">
@@ -2751,14 +2730,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
       <c r="A2" s="9" t="s">
@@ -4886,10 +4865,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="40"/>
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1">
       <c r="A2" s="12" t="s">
@@ -4927,10 +4906,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="41"/>
+      <c r="B7" s="40"/>
     </row>
     <row r="8" spans="1:3" ht="12.75" customHeight="1">
       <c r="A8" s="12" t="s">
@@ -5955,15 +5934,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
@@ -33738,62 +33717,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="44"/>
+      <c r="D2" s="43"/>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="44" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="44"/>
+      <c r="D3" s="43"/>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="44" t="s">
+      <c r="B4" s="42"/>
+      <c r="C4" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="44"/>
+      <c r="D4" s="43"/>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44" t="s">
+      <c r="B5" s="42"/>
+      <c r="C5" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="44"/>
+      <c r="D5" s="43"/>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="44" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="44"/>
+      <c r="D6" s="43"/>
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1">
       <c r="A8" s="6" t="s">
@@ -34856,12 +34835,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1">
       <c r="A2" s="6" t="s">

</xml_diff>